<commit_message>
2: Deadlock simulations, fixes
</commit_message>
<xml_diff>
--- a/test_results/Statistics.xlsx
+++ b/test_results/Statistics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\deadlock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\deadlock\test_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1220C5-6474-4F2F-93B9-7DA9BE808A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FAEFD2-3237-4526-84AB-7EF5C765956F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B8E184BE-C930-4626-BBA9-56E66D6AA4EC}"/>
   </bookViews>
@@ -305,27 +305,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -343,16 +323,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -678,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68016524-E6AB-4BCF-AB22-79EC0E7ADE81}">
   <dimension ref="B1:AF22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,7 +1105,7 @@
         <v>31</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>0</v>
@@ -1322,7 +1292,7 @@
         <v>31</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>31</v>
@@ -1420,7 +1390,7 @@
         <v>31</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>0</v>
@@ -1987,7 +1957,7 @@
         <v>31</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>31</v>
@@ -2079,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>31</v>
@@ -2652,7 +2622,7 @@
         <v>31</v>
       </c>
       <c r="P22" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q22" s="9" t="s">
         <v>31</v>
@@ -2705,13 +2675,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:AF22">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Incorrect"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Deadlock"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>